<commit_message>
Automatische test-sync: 2025-07-31 21:23:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,8 +735,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij dit even regelen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:23:08</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -756,7 +808,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -764,17 +816,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,7 +868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wil je dit oppakken?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:25:23</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,17 +868,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -841,7 +893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,6 +923,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:27:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,8 +839,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #3: Kun jij dit afhandelen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:27:34</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -860,7 +912,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -868,17 +920,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -920,7 +972,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:32:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,8 +946,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wil je deze klant bellen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:32:10</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -967,7 +1019,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -975,17 +1027,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1037,7 +1089,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,8 +1053,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #7: Is dit artikel nog op voorraad?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:36:52</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1074,7 +1126,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1082,17 +1134,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1150,17 +1202,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1160,8 +1160,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #9: Hoi, hebben jullie al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:41:15</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1181,7 +1233,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1189,17 +1241,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1241,7 +1293,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1212,8 +1212,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #10: Is er al nieuws?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:43:42</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1233,7 +1285,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1241,17 +1293,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1293,7 +1345,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1486,8 +1486,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #15: Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:54:44</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1507,7 +1559,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1515,17 +1567,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1587,7 +1639,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 21:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,8 +1538,60 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wil je dit even doorsturen?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-07-31 21:56:55</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1559,7 +1611,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1567,17 +1619,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1639,7 +1691,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 22:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1701,8 +1701,60 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #19: Bel jij klant Jansen even?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-07-31 22:04:06</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1722,7 +1774,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1730,17 +1782,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1788,7 +1840,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1798,11 +1850,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-31 22:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-31.xlsx
+++ b/logs/mail_log_2025-07-31.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1753,8 +1753,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #20: Ik ben niet tevreden over hoe dit is gegaan.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Dank voor je bericht. We pakken dit intern op en houden je op de hoogte.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-07-31 22:06:18</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1774,7 +1826,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1782,17 +1834,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1807,7 +1859,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,6 +1939,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>